<commit_message>
feat: 🎸 Ajuste de Horton
</commit_message>
<xml_diff>
--- a/backend/taxa_inf.xlsx
+++ b/backend/taxa_inf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mestrado\Trabalho Final\Codigos\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9559C0-B0BA-4368-8711-F8F411F30592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9AD5F80-3B64-417A-91C8-D7908374CDB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ajuste" sheetId="2" r:id="rId1"/>
@@ -1237,7 +1237,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0E+00"/>
+    <numFmt numFmtId="164" formatCode="0.0E+00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -1640,18 +1640,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1869,46 +1869,46 @@
                 <c:formatCode>0.0E+00</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="1">
-                  <c:v>3.1797865841460859E-7</c:v>
+                  <c:v>2.3848399381095652E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.589893292073043E-7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1.589893292073043E-7</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>1.589893292073043E-7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.589893292073043E-7</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.9494664603652148E-8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.9494664603652148E-8</c:v>
+                  <c:v>1.589893292073043E-7</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.9494664603652148E-8</c:v>
+                  <c:v>1.589893292073043E-7</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>1.589893292073043E-7</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>7.9494664603652148E-8</c:v>
@@ -1917,16 +1917,16 @@
                   <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>1.589893292073043E-7</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>1.589893292073043E-7</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>7.9494664603652148E-8</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2051,16 +2051,16 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>11</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>11</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>11</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>11</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2072,82 +2072,82 @@
                 <c:formatCode>0.0E+00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>2.8765859524327411E-5</c:v>
+                  <c:v>2.88853915022535E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.1801875392468344E-7</c:v>
+                  <c:v>2.3127176120424046E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.1614634850587013E-8</c:v>
+                  <c:v>1.8921752280074319E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.9303630904496212E-8</c:v>
+                  <c:v>1.5850385805525579E-7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.9282801522900737E-8</c:v>
+                  <c:v>1.3607260646422123E-7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.9282613784953169E-8</c:v>
+                  <c:v>1.1969028764587775E-7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.9282612092846435E-8</c:v>
+                  <c:v>1.0772571363284684E-7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.928261207759525E-8</c:v>
+                  <c:v>9.8987571438165146E-8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.9282612077457792E-8</c:v>
+                  <c:v>9.2605803986075644E-8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.9282612077456555E-8</c:v>
+                  <c:v>8.7944978503361886E-8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>8.4541016459398425E-8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>8.2054985253184422E-8</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>8.0239350684276698E-8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.8913329965159079E-8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.7944891173763385E-8</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.7237606831099404E-8</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.6721052614330914E-8</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.6343795204876183E-8</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.6068271071361487E-8</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.5867046267695626E-8</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.5720084834249333E-8</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.5534366262668951E-8</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.5339253103689209E-8</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.5324676978613504E-8</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.5323460217819479E-8</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.5322811211475918E-8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2548,7 +2548,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>P97</c:v>
+                  <c:v>P162</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2582,46 +2582,46 @@
                 <c:formatCode>0.0E+00</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="1">
-                  <c:v>3.1797865841460859E-7</c:v>
+                  <c:v>2.3848399381095652E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.589893292073043E-7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1.589893292073043E-7</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>1.589893292073043E-7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.589893292073043E-7</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.9494664603652148E-8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.9494664603652148E-8</c:v>
+                  <c:v>1.589893292073043E-7</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.9494664603652148E-8</c:v>
+                  <c:v>1.589893292073043E-7</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>1.589893292073043E-7</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>7.9494664603652148E-8</c:v>
@@ -2630,16 +2630,16 @@
                   <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>1.589893292073043E-7</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>1.589893292073043E-7</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>7.9494664603652148E-8</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2651,67 +2651,67 @@
                 <c:formatCode>0.0E+00</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>2.8765859524327411E-5</c:v>
+                  <c:v>2.88853915022535E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.1801875392468344E-7</c:v>
+                  <c:v>2.3127176120424046E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.1614634850587013E-8</c:v>
+                  <c:v>1.8921752280074319E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.9303630904496212E-8</c:v>
+                  <c:v>1.5850385805525579E-7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.9282801522900737E-8</c:v>
+                  <c:v>1.3607260646422123E-7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.9282613784953169E-8</c:v>
+                  <c:v>1.1969028764587775E-7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.9282612092846435E-8</c:v>
+                  <c:v>1.0772571363284684E-7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.928261207759525E-8</c:v>
+                  <c:v>9.8987571438165146E-8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.9282612077457792E-8</c:v>
+                  <c:v>9.2605803986075644E-8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.9282612077456555E-8</c:v>
+                  <c:v>8.7944978503361886E-8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>8.4541016459398425E-8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>8.2054985253184422E-8</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>8.0239350684276698E-8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.8913329965159079E-8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.7944891173763385E-8</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.7237606831099404E-8</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.6721052614330914E-8</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.6343795204876183E-8</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.6068271071361487E-8</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.5867046267695626E-8</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.5720084834249333E-8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3212,46 +3212,46 @@
                 <c:formatCode>0.0E+00</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="1">
-                  <c:v>3.1797865841460859E-7</c:v>
+                  <c:v>2.3848399381095652E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.589893292073043E-7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1.589893292073043E-7</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>1.589893292073043E-7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.589893292073043E-7</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.9494664603652148E-8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.9494664603652148E-8</c:v>
+                  <c:v>1.589893292073043E-7</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.9494664603652148E-8</c:v>
+                  <c:v>1.589893292073043E-7</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>1.589893292073043E-7</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>7.9494664603652148E-8</c:v>
@@ -3260,16 +3260,16 @@
                   <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>1.589893292073043E-7</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>1.589893292073043E-7</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>7.9494664603652148E-8</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3394,16 +3394,16 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>11</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>11</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>11</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>11</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3415,82 +3415,82 @@
                 <c:formatCode>0.0E+00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>2.8765859524327411E-5</c:v>
+                  <c:v>2.88853915022535E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.1801875392468344E-7</c:v>
+                  <c:v>2.3127176120424046E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.1614634850587013E-8</c:v>
+                  <c:v>1.8921752280074319E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.9303630904496212E-8</c:v>
+                  <c:v>1.5850385805525579E-7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.9282801522900737E-8</c:v>
+                  <c:v>1.3607260646422123E-7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.9282613784953169E-8</c:v>
+                  <c:v>1.1969028764587775E-7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.9282612092846435E-8</c:v>
+                  <c:v>1.0772571363284684E-7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.928261207759525E-8</c:v>
+                  <c:v>9.8987571438165146E-8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.9282612077457792E-8</c:v>
+                  <c:v>9.2605803986075644E-8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.9282612077456555E-8</c:v>
+                  <c:v>8.7944978503361886E-8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>8.4541016459398425E-8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>8.2054985253184422E-8</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>8.0239350684276698E-8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.8913329965159079E-8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.7944891173763385E-8</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.7237606831099404E-8</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.6721052614330914E-8</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.6343795204876183E-8</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.6068271071361487E-8</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.5867046267695626E-8</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.5720084834249333E-8</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.5534366262668951E-8</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.5339253103689209E-8</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.5324676978613504E-8</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.5323460217819479E-8</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.5322811211475918E-8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3891,7 +3891,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>P97</c:v>
+                  <c:v>P162</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4003,46 +4003,46 @@
                 <c:formatCode>0.0E+00</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="1">
-                  <c:v>3.1797865841460859E-7</c:v>
+                  <c:v>2.3848399381095652E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.589893292073043E-7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1.589893292073043E-7</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>1.589893292073043E-7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.589893292073043E-7</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.9494664603652148E-8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.9494664603652148E-8</c:v>
+                  <c:v>1.589893292073043E-7</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.9494664603652148E-8</c:v>
+                  <c:v>1.589893292073043E-7</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>1.589893292073043E-7</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>7.9494664603652148E-8</c:v>
@@ -4051,16 +4051,16 @@
                   <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>1.589893292073043E-7</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>7.9494664603652148E-8</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>1.589893292073043E-7</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>7.9494664603652148E-8</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4072,67 +4072,67 @@
                 <c:formatCode>0.0E+00</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>2.8765859524327411E-5</c:v>
+                  <c:v>2.88853915022535E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.1801875392468344E-7</c:v>
+                  <c:v>2.3127176120424046E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.1614634850587013E-8</c:v>
+                  <c:v>1.8921752280074319E-7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.9303630904496212E-8</c:v>
+                  <c:v>1.5850385805525579E-7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.9282801522900737E-8</c:v>
+                  <c:v>1.3607260646422123E-7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.9282613784953169E-8</c:v>
+                  <c:v>1.1969028764587775E-7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.9282612092846435E-8</c:v>
+                  <c:v>1.0772571363284684E-7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.928261207759525E-8</c:v>
+                  <c:v>9.8987571438165146E-8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.9282612077457792E-8</c:v>
+                  <c:v>9.2605803986075644E-8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.9282612077456555E-8</c:v>
+                  <c:v>8.7944978503361886E-8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>8.4541016459398425E-8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>8.2054985253184422E-8</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>8.0239350684276698E-8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.8913329965159079E-8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.7944891173763385E-8</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.7237606831099404E-8</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.6721052614330914E-8</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.6343795204876183E-8</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.6068271071361487E-8</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.5867046267695626E-8</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.9282612077456542E-8</c:v>
+                  <c:v>7.5720084834249333E-8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6749,15 +6749,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>41</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>51</xdr:col>
-      <xdr:colOff>333377</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>23814</xdr:rowOff>
+      <xdr:colOff>510542</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>151449</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6787,15 +6787,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>51</xdr:col>
-      <xdr:colOff>590549</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>493394</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>158115</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>60</xdr:col>
-      <xdr:colOff>523874</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>426719</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>182880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7112,8 +7112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0473EC8C-1C4A-4349-AAD0-922A5F5E33BB}">
   <dimension ref="B1:I31"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7134,7 +7134,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>207</v>
+        <v>361</v>
       </c>
       <c r="D2"/>
       <c r="E2" s="3" t="str">
@@ -7159,24 +7159,24 @@
       </c>
       <c r="C3" s="19">
         <f>MATCH($C$2,Dados!$A$2:$A$87,0)+1</f>
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="D3"/>
       <c r="E3" s="6">
         <f>HLOOKUP(E2,Dados!$AM$1:$AO$87,$C$3,FALSE)</f>
-        <v>5.9282612077456542E-8</v>
+        <v>7.5322069325201654E-8</v>
       </c>
       <c r="F3" s="12">
         <f>HLOOKUP(F2,Dados!$AM$1:$AO$87,$C$3,FALSE)</f>
-        <v>2.8765859524327411E-5</v>
+        <v>2.88853915022535E-7</v>
       </c>
       <c r="G3" s="7">
         <f>HLOOKUP(G2,Dados!$AM$1:$AO$87,$C$3,FALSE)</f>
-        <v>9.4181455022660767</v>
+        <v>0.62850502887206972</v>
       </c>
       <c r="I3" s="21">
         <f>RSQ(C7:C26,D7:D26)</f>
-        <v>0.62437284061868081</v>
+        <v>0.24216667566189012</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -7198,7 +7198,7 @@
       <c r="C6" s="24"/>
       <c r="D6" s="26">
         <f t="shared" ref="D6:D31" si="0">$E$3+($F$3-$E$3)*EXP(-$G$3*B6)</f>
-        <v>2.8765859524327411E-5</v>
+        <v>2.88853915022535E-7</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
@@ -7207,11 +7207,11 @@
       </c>
       <c r="C7" s="25">
         <f>HLOOKUP(B7,Dados!$AQ$1:$BJ$87,$C$3,FALSE)</f>
-        <v>3.1797865841460859E-7</v>
+        <v>2.3848399381095652E-7</v>
       </c>
       <c r="D7" s="26">
         <f t="shared" si="0"/>
-        <v>3.1801875392468344E-7</v>
+        <v>2.3127176120424046E-7</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
@@ -7220,11 +7220,11 @@
       </c>
       <c r="C8" s="25">
         <f>HLOOKUP(B8,Dados!$AQ$1:$BJ$87,$C$3,FALSE)</f>
-        <v>0</v>
+        <v>7.9494664603652148E-8</v>
       </c>
       <c r="D8" s="26">
         <f t="shared" si="0"/>
-        <v>6.1614634850587013E-8</v>
+        <v>1.8921752280074319E-7</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
@@ -7237,7 +7237,7 @@
       </c>
       <c r="D9" s="26">
         <f t="shared" si="0"/>
-        <v>5.9303630904496212E-8</v>
+        <v>1.5850385805525579E-7</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
@@ -7246,11 +7246,11 @@
       </c>
       <c r="C10" s="25">
         <f>HLOOKUP(B10,Dados!$AQ$1:$BJ$87,$C$3,FALSE)</f>
-        <v>0</v>
+        <v>1.589893292073043E-7</v>
       </c>
       <c r="D10" s="26">
         <f t="shared" si="0"/>
-        <v>5.9282801522900737E-8</v>
+        <v>1.3607260646422123E-7</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
@@ -7259,11 +7259,11 @@
       </c>
       <c r="C11" s="25">
         <f>HLOOKUP(B11,Dados!$AQ$1:$BJ$87,$C$3,FALSE)</f>
-        <v>7.9494664603652148E-8</v>
+        <v>1.589893292073043E-7</v>
       </c>
       <c r="D11" s="26">
         <f t="shared" si="0"/>
-        <v>5.9282613784953169E-8</v>
+        <v>1.1969028764587775E-7</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
@@ -7272,11 +7272,11 @@
       </c>
       <c r="C12" s="25">
         <f>HLOOKUP(B12,Dados!$AQ$1:$BJ$87,$C$3,FALSE)</f>
-        <v>7.9494664603652148E-8</v>
+        <v>1.589893292073043E-7</v>
       </c>
       <c r="D12" s="26">
         <f t="shared" si="0"/>
-        <v>5.9282612092846435E-8</v>
+        <v>1.0772571363284684E-7</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
@@ -7285,11 +7285,11 @@
       </c>
       <c r="C13" s="25">
         <f>HLOOKUP(B13,Dados!$AQ$1:$BJ$87,$C$3,FALSE)</f>
-        <v>0</v>
+        <v>7.9494664603652148E-8</v>
       </c>
       <c r="D13" s="26">
         <f t="shared" si="0"/>
-        <v>5.928261207759525E-8</v>
+        <v>9.8987571438165146E-8</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
@@ -7298,11 +7298,11 @@
       </c>
       <c r="C14" s="25">
         <f>HLOOKUP(B14,Dados!$AQ$1:$BJ$87,$C$3,FALSE)</f>
-        <v>7.9494664603652148E-8</v>
+        <v>1.589893292073043E-7</v>
       </c>
       <c r="D14" s="26">
         <f t="shared" si="0"/>
-        <v>5.9282612077457792E-8</v>
+        <v>9.2605803986075644E-8</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
@@ -7315,7 +7315,7 @@
       </c>
       <c r="D15" s="26">
         <f t="shared" si="0"/>
-        <v>5.9282612077456555E-8</v>
+        <v>8.7944978503361886E-8</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
@@ -7324,11 +7324,11 @@
       </c>
       <c r="C16" s="25">
         <f>HLOOKUP(B16,Dados!$AQ$1:$BJ$87,$C$3,FALSE)</f>
-        <v>0</v>
+        <v>7.9494664603652148E-8</v>
       </c>
       <c r="D16" s="26">
         <f t="shared" si="0"/>
-        <v>5.9282612077456542E-8</v>
+        <v>8.4541016459398425E-8</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
@@ -7337,11 +7337,11 @@
       </c>
       <c r="C17" s="25">
         <f>HLOOKUP(B17,Dados!$AQ$1:$BJ$87,$C$3,FALSE)</f>
-        <v>7.9494664603652148E-8</v>
+        <v>1.589893292073043E-7</v>
       </c>
       <c r="D17" s="26">
         <f t="shared" si="0"/>
-        <v>5.9282612077456542E-8</v>
+        <v>8.2054985253184422E-8</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
@@ -7354,7 +7354,7 @@
       </c>
       <c r="D18" s="26">
         <f t="shared" si="0"/>
-        <v>5.9282612077456542E-8</v>
+        <v>8.0239350684276698E-8</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
@@ -7363,11 +7363,11 @@
       </c>
       <c r="C19" s="25">
         <f>HLOOKUP(B19,Dados!$AQ$1:$BJ$87,$C$3,FALSE)</f>
-        <v>0</v>
+        <v>1.589893292073043E-7</v>
       </c>
       <c r="D19" s="26">
         <f t="shared" si="0"/>
-        <v>5.9282612077456542E-8</v>
+        <v>7.8913329965159079E-8</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
@@ -7376,11 +7376,11 @@
       </c>
       <c r="C20" s="25">
         <f>HLOOKUP(B20,Dados!$AQ$1:$BJ$87,$C$3,FALSE)</f>
-        <v>0</v>
+        <v>7.9494664603652148E-8</v>
       </c>
       <c r="D20" s="26">
         <f t="shared" si="0"/>
-        <v>5.9282612077456542E-8</v>
+        <v>7.7944891173763385E-8</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
@@ -7393,7 +7393,7 @@
       </c>
       <c r="D21" s="26">
         <f t="shared" si="0"/>
-        <v>5.9282612077456542E-8</v>
+        <v>7.7237606831099404E-8</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
@@ -7406,7 +7406,7 @@
       </c>
       <c r="D22" s="26">
         <f t="shared" si="0"/>
-        <v>5.9282612077456542E-8</v>
+        <v>7.6721052614330914E-8</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
@@ -7415,11 +7415,11 @@
       </c>
       <c r="C23" s="25">
         <f>HLOOKUP(B23,Dados!$AQ$1:$BJ$87,$C$3,FALSE)</f>
-        <v>0</v>
+        <v>1.589893292073043E-7</v>
       </c>
       <c r="D23" s="26">
         <f t="shared" si="0"/>
-        <v>5.9282612077456542E-8</v>
+        <v>7.6343795204876183E-8</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
@@ -7428,11 +7428,11 @@
       </c>
       <c r="C24" s="25">
         <f>HLOOKUP(B24,Dados!$AQ$1:$BJ$87,$C$3,FALSE)</f>
-        <v>0</v>
+        <v>7.9494664603652148E-8</v>
       </c>
       <c r="D24" s="26">
         <f t="shared" si="0"/>
-        <v>5.9282612077456542E-8</v>
+        <v>7.6068271071361487E-8</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
@@ -7441,11 +7441,11 @@
       </c>
       <c r="C25" s="25">
         <f>HLOOKUP(B25,Dados!$AQ$1:$BJ$87,$C$3,FALSE)</f>
-        <v>7.9494664603652148E-8</v>
+        <v>1.589893292073043E-7</v>
       </c>
       <c r="D25" s="26">
         <f t="shared" si="0"/>
-        <v>5.9282612077456542E-8</v>
+        <v>7.5867046267695626E-8</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
@@ -7454,11 +7454,11 @@
       </c>
       <c r="C26" s="25">
         <f>HLOOKUP(B26,Dados!$AQ$1:$BJ$87,$C$3,FALSE)</f>
-        <v>0</v>
+        <v>7.9494664603652148E-8</v>
       </c>
       <c r="D26" s="26">
         <f t="shared" si="0"/>
-        <v>5.9282612077456542E-8</v>
+        <v>7.5720084834249333E-8</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
@@ -7468,47 +7468,47 @@
       <c r="C27" s="27"/>
       <c r="D27" s="26">
         <f t="shared" si="0"/>
-        <v>5.9282612077456542E-8</v>
+        <v>7.5534366262668951E-8</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="22">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C28" s="27"/>
       <c r="D28" s="26">
         <f t="shared" si="0"/>
-        <v>5.9282612077456542E-8</v>
+        <v>7.5339253103689209E-8</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="22">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C29" s="27"/>
       <c r="D29" s="26">
         <f t="shared" si="0"/>
-        <v>5.9282612077456542E-8</v>
+        <v>7.5324676978613504E-8</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="22">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C30" s="27"/>
       <c r="D30" s="26">
         <f t="shared" si="0"/>
-        <v>5.9282612077456542E-8</v>
+        <v>7.5323460217819479E-8</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="23">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C31" s="28"/>
       <c r="D31" s="29">
         <f t="shared" si="0"/>
-        <v>5.9282612077456542E-8</v>
+        <v>7.5322811211475918E-8</v>
       </c>
     </row>
   </sheetData>
@@ -7533,11 +7533,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BJ87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AJ37" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AO47" sqref="AO47"/>
+      <selection pane="bottomRight" activeCell="AN87" sqref="AN87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15309,10 +15309,10 @@
         <v>5.9282612077456542E-8</v>
       </c>
       <c r="AN47" s="1">
-        <v>2.8765859524327411E-5</v>
+        <v>4.9999999999999998E-7</v>
       </c>
       <c r="AO47" s="1">
-        <v>9.4181455022660767</v>
+        <v>1.2</v>
       </c>
       <c r="AQ47" s="1">
         <v>3.1797865841460859E-7</v>
@@ -15806,14 +15806,14 @@
       <c r="AK50" s="1">
         <v>1.0185185185185189E-2</v>
       </c>
-      <c r="AM50" s="1">
-        <v>1.713570352865786E-11</v>
-      </c>
-      <c r="AN50" s="1">
-        <v>1.3113081415916429E-5</v>
+      <c r="AM50" s="14">
+        <v>2.9999999999999997E-8</v>
+      </c>
+      <c r="AN50" s="14">
+        <v>1.3113081415916401E-6</v>
       </c>
       <c r="AO50" s="1">
-        <v>8.8275112970457386</v>
+        <v>2</v>
       </c>
       <c r="AQ50" s="1">
         <v>1.589893292073043E-7</v>
@@ -16140,14 +16140,14 @@
       <c r="AK52" s="1">
         <v>0.17450980392156859</v>
       </c>
-      <c r="AM52" s="1">
-        <v>7.0371804138870749E-7</v>
-      </c>
-      <c r="AN52" s="1">
-        <v>2.787537762974015E-6</v>
+      <c r="AM52" s="14">
+        <v>3.9999999999999998E-7</v>
+      </c>
+      <c r="AN52" s="14">
+        <v>1.9999999999999999E-6</v>
       </c>
       <c r="AO52" s="1">
-        <v>1.538497774651773</v>
+        <v>0.7</v>
       </c>
       <c r="AQ52" s="1">
         <v>1.748882621280347E-6</v>
@@ -16385,55 +16385,55 @@
         <v>90</v>
       </c>
       <c r="C54" s="1">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="D54" s="1">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="E54" s="1">
-        <v>65</v>
+        <v>86.5</v>
       </c>
       <c r="F54" s="1">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="G54" s="1">
-        <v>65</v>
+        <v>84.5</v>
       </c>
       <c r="H54" s="1">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="I54" s="1">
-        <v>65</v>
+        <v>81.5</v>
       </c>
       <c r="J54" s="1">
-        <v>65</v>
+        <v>80.5</v>
       </c>
       <c r="K54" s="1">
-        <v>65</v>
+        <v>79.5</v>
       </c>
       <c r="L54" s="1">
-        <v>65</v>
+        <v>78.5</v>
       </c>
       <c r="M54" s="1">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="N54" s="1">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="O54" s="1">
-        <v>65</v>
+        <v>74.5</v>
       </c>
       <c r="P54" s="1">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="Q54" s="1">
-        <v>65</v>
+        <v>72.5</v>
       </c>
       <c r="R54" s="1">
-        <v>65</v>
+        <v>71.5</v>
       </c>
       <c r="S54" s="1">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="T54" s="1">
         <v>67.5</v>
@@ -16474,74 +16474,74 @@
       <c r="AK54" s="1">
         <v>4.1666666666666657E-2</v>
       </c>
-      <c r="AM54" s="1">
-        <v>8.7078975601839405E-11</v>
-      </c>
-      <c r="AN54" s="1">
-        <v>2.7848192970323201E-4</v>
+      <c r="AM54" s="14">
+        <v>1.9173400394398601E-7</v>
+      </c>
+      <c r="AN54" s="14">
+        <v>1.6258064242463301E-6</v>
       </c>
       <c r="AO54" s="1">
-        <v>8.4992123177331358</v>
-      </c>
-      <c r="AQ54" s="1">
-        <v>3.9747332301826066E-6</v>
-      </c>
-      <c r="AR54" s="1">
-        <v>0</v>
-      </c>
-      <c r="AS54" s="1">
-        <v>0</v>
-      </c>
-      <c r="AT54" s="1">
-        <v>0</v>
-      </c>
-      <c r="AU54" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV54" s="1">
-        <v>0</v>
-      </c>
-      <c r="AW54" s="1">
-        <v>0</v>
-      </c>
-      <c r="AX54" s="1">
-        <v>0</v>
-      </c>
-      <c r="AY54" s="1">
-        <v>0</v>
-      </c>
-      <c r="AZ54" s="1">
-        <v>0</v>
-      </c>
-      <c r="BA54" s="1">
-        <v>0</v>
-      </c>
-      <c r="BB54" s="1">
-        <v>0</v>
-      </c>
-      <c r="BC54" s="1">
-        <v>0</v>
-      </c>
-      <c r="BD54" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE54" s="1">
-        <v>0</v>
-      </c>
-      <c r="BF54" s="1">
-        <v>0</v>
-      </c>
-      <c r="BG54" s="1">
-        <v>0</v>
-      </c>
-      <c r="BH54" s="1">
-        <v>-3.9747332301826072E-7</v>
-      </c>
-      <c r="BI54" s="1">
-        <v>2.3848399381095652E-7</v>
-      </c>
-      <c r="BJ54" s="1">
-        <v>1.589893292073043E-7</v>
+        <v>3</v>
+      </c>
+      <c r="AQ54" s="14">
+        <v>1.5898932920730401E-7</v>
+      </c>
+      <c r="AR54" s="14">
+        <v>1.5898932920730401E-7</v>
+      </c>
+      <c r="AS54" s="14">
+        <v>2.38483993810956E-7</v>
+      </c>
+      <c r="AT54" s="14">
+        <v>2.38483993810956E-7</v>
+      </c>
+      <c r="AU54" s="14">
+        <v>7.9494664603652095E-8</v>
+      </c>
+      <c r="AV54" s="14">
+        <v>2.38483993810956E-7</v>
+      </c>
+      <c r="AW54" s="14">
+        <v>2.38483993810956E-7</v>
+      </c>
+      <c r="AX54" s="14">
+        <v>1.5898932920730401E-7</v>
+      </c>
+      <c r="AY54" s="14">
+        <v>1.5898932920730401E-7</v>
+      </c>
+      <c r="AZ54" s="14">
+        <v>1.5898932920730401E-7</v>
+      </c>
+      <c r="BA54" s="14">
+        <v>2.38483993810956E-7</v>
+      </c>
+      <c r="BB54" s="14">
+        <v>1.5898932920730401E-7</v>
+      </c>
+      <c r="BC54" s="14">
+        <v>2.38483993810956E-7</v>
+      </c>
+      <c r="BD54" s="14">
+        <v>2.38483993810956E-7</v>
+      </c>
+      <c r="BE54" s="14">
+        <v>7.9494664603652095E-8</v>
+      </c>
+      <c r="BF54" s="14">
+        <v>1.5898932920730401E-7</v>
+      </c>
+      <c r="BG54" s="14">
+        <v>3.9747332301825997E-7</v>
+      </c>
+      <c r="BH54" s="14">
+        <v>2.38483993810956E-7</v>
+      </c>
+      <c r="BI54" s="14">
+        <v>2.38483993810956E-7</v>
+      </c>
+      <c r="BJ54" s="14">
+        <v>1.5898932920730401E-7</v>
       </c>
     </row>
     <row r="55" spans="1:62" x14ac:dyDescent="0.25">
@@ -16975,14 +16975,14 @@
       <c r="AK57" s="1">
         <v>3.508771929824561E-3</v>
       </c>
-      <c r="AM57" s="1">
-        <v>1.163192005441873E-12</v>
-      </c>
-      <c r="AN57" s="1">
-        <v>1.0583570858957741E-5</v>
+      <c r="AM57" s="14">
+        <v>1.1631920054418699E-8</v>
+      </c>
+      <c r="AN57" s="14">
+        <v>4.9999999999999998E-7</v>
       </c>
       <c r="AO57" s="1">
-        <v>8.3963985917078574</v>
+        <v>5</v>
       </c>
       <c r="AQ57" s="1">
         <v>1.589893292073043E-7</v>
@@ -17142,14 +17142,14 @@
       <c r="AK58" s="1">
         <v>1.666666666666667E-3</v>
       </c>
-      <c r="AM58" s="1">
-        <v>1.9208427784578522E-12</v>
-      </c>
-      <c r="AN58" s="1">
-        <v>7.645382338899509E-6</v>
+      <c r="AM58" s="14">
+        <v>1.9208427784578499E-10</v>
+      </c>
+      <c r="AN58" s="14">
+        <v>7.6453823388995098E-7</v>
       </c>
       <c r="AO58" s="1">
-        <v>9.1392033093069678</v>
+        <v>5</v>
       </c>
       <c r="AQ58" s="1">
         <v>7.9494664603652148E-8</v>
@@ -17718,10 +17718,10 @@
         <v>267</v>
       </c>
       <c r="B62" s="1">
+        <v>95</v>
+      </c>
+      <c r="C62" s="1">
         <v>91</v>
-      </c>
-      <c r="C62" s="1">
-        <v>7</v>
       </c>
       <c r="D62" s="1">
         <v>81</v>
@@ -17810,20 +17810,20 @@
       <c r="AK62" s="1">
         <v>0.14000000000000001</v>
       </c>
-      <c r="AM62" s="1">
+      <c r="AM62" s="14">
         <v>6.3508091863586201E-7</v>
       </c>
-      <c r="AN62" s="1">
-        <v>1.2620742862134451E-3</v>
+      <c r="AN62" s="14">
+        <v>3.0000000000000001E-6</v>
       </c>
       <c r="AO62" s="1">
-        <v>9.1941669610460899</v>
-      </c>
-      <c r="AQ62" s="1">
-        <v>1.335510365341356E-5</v>
-      </c>
-      <c r="AR62" s="1">
-        <v>-1.1765210361340519E-5</v>
+        <v>2.5</v>
+      </c>
+      <c r="AQ62" s="14">
+        <v>6.3595731679999995E-7</v>
+      </c>
+      <c r="AR62" s="14">
+        <v>1.589893292E-6</v>
       </c>
       <c r="AS62" s="1">
         <v>4.7696798762191305E-7</v>
@@ -18311,14 +18311,14 @@
       <c r="AK65" s="1">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AM65" s="1">
-        <v>9.989102473964456E-12</v>
+      <c r="AM65" s="14">
+        <v>4.9999999999999998E-8</v>
       </c>
       <c r="AN65" s="1">
-        <v>3.1373986860224499E-5</v>
+        <v>3.0000000000000001E-6</v>
       </c>
       <c r="AO65" s="1">
-        <v>8.3727355873260745</v>
+        <v>5</v>
       </c>
       <c r="AQ65" s="1">
         <v>4.7696798762191305E-7</v>
@@ -19146,14 +19146,14 @@
       <c r="AK70" s="1">
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="AM70" s="1">
-        <v>5.3378110541612192E-11</v>
-      </c>
-      <c r="AN70" s="1">
-        <v>0</v>
+      <c r="AM70" s="14">
+        <v>5.3378110541612203E-9</v>
+      </c>
+      <c r="AN70" s="14">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="AO70" s="1">
-        <v>74.269206129716196</v>
+        <v>2</v>
       </c>
       <c r="AQ70" s="1">
         <v>0</v>
@@ -19647,8 +19647,8 @@
       <c r="AK73" s="1">
         <v>1.5833333333333331E-2</v>
       </c>
-      <c r="AM73" s="1">
-        <v>7.4604167027713245E-8</v>
+      <c r="AM73" s="14">
+        <v>4.8460416702771297E-8</v>
       </c>
       <c r="AN73" s="1">
         <v>2.345221669568882E-7</v>
@@ -19814,14 +19814,14 @@
       <c r="AK74" s="1">
         <v>0.01</v>
       </c>
-      <c r="AM74" s="1">
-        <v>4.2930345529971477E-12</v>
+      <c r="AM74" s="14">
+        <v>4.9999999999999998E-8</v>
       </c>
       <c r="AN74" s="1">
-        <v>1.2261056361579249E-5</v>
+        <v>1.2261056361579201E-6</v>
       </c>
       <c r="AO74" s="1">
-        <v>8.6918195915725693</v>
+        <v>5</v>
       </c>
       <c r="AQ74" s="1">
         <v>1.589893292073043E-7</v>
@@ -19981,14 +19981,14 @@
       <c r="AK75" s="1">
         <v>0.16666666666666671</v>
       </c>
-      <c r="AM75" s="1">
-        <v>5.3543030216332681E-7</v>
-      </c>
-      <c r="AN75" s="1">
-        <v>1.0622929054008791E-6</v>
+      <c r="AM75" s="14">
+        <v>6.5000000000000002E-7</v>
+      </c>
+      <c r="AN75" s="14">
+        <v>8.0622929054008802E-6</v>
       </c>
       <c r="AO75" s="1">
-        <v>0.28591358650197662</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="AQ75" s="1">
         <v>7.9494664603652143E-7</v>
@@ -20309,14 +20309,14 @@
       <c r="AK77" s="1">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AM77" s="1">
-        <v>6.7681947112294867E-8</v>
-      </c>
-      <c r="AN77" s="1">
-        <v>1.7547785770977281E-7</v>
+      <c r="AM77" s="14">
+        <v>1.1999999999999999E-7</v>
+      </c>
+      <c r="AN77" s="14">
+        <v>1.75477857709773E-6</v>
       </c>
       <c r="AO77" s="1">
-        <v>0.14278938490451759</v>
+        <v>6</v>
       </c>
       <c r="AQ77" s="1">
         <v>1.589893292073043E-7</v>
@@ -20476,14 +20476,14 @@
       <c r="AK78" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AM78" s="1">
-        <v>3.1799051282747009E-7</v>
+      <c r="AM78" s="14">
+        <v>3.2000000000000001E-7</v>
       </c>
       <c r="AN78" s="1">
-        <v>3.8323374526453279E-5</v>
+        <v>3.0000000000000001E-6</v>
       </c>
       <c r="AO78" s="1">
-        <v>9.5674868978940957</v>
+        <v>5</v>
       </c>
       <c r="AQ78" s="1">
         <v>6.3595731682921719E-7</v>
@@ -20718,61 +20718,61 @@
         <v>89</v>
       </c>
       <c r="C80" s="1">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="D80" s="1">
-        <v>63</v>
+        <v>87.5</v>
       </c>
       <c r="E80" s="1">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="F80" s="1">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="G80" s="1">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="H80" s="1">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="I80" s="1">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="J80" s="1">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="K80" s="1">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="L80" s="1">
-        <v>63</v>
+        <v>78.5</v>
       </c>
       <c r="M80" s="1">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="N80" s="1">
-        <v>63</v>
+        <v>75.5</v>
       </c>
       <c r="O80" s="1">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="P80" s="1">
-        <v>63</v>
+        <v>72.5</v>
       </c>
       <c r="Q80" s="1">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="R80" s="1">
-        <v>63</v>
+        <v>69.5</v>
       </c>
       <c r="S80" s="1">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="T80" s="1">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="U80" s="1">
-        <v>63</v>
+        <v>64.5</v>
       </c>
       <c r="V80" s="1">
         <v>63</v>
@@ -20804,74 +20804,74 @@
       <c r="AK80" s="1">
         <v>4.3333333333333328E-2</v>
       </c>
-      <c r="AM80" s="1">
-        <v>9.9269113003885896E-11</v>
-      </c>
-      <c r="AN80" s="1">
-        <v>3.7422035262075522E-4</v>
+      <c r="AM80" s="14">
+        <v>1.8E-7</v>
+      </c>
+      <c r="AN80" s="14">
+        <v>1.7422035262075501E-6</v>
       </c>
       <c r="AO80" s="1">
-        <v>9.0120785113650541</v>
-      </c>
-      <c r="AQ80" s="1">
-        <v>4.1337225593899122E-6</v>
-      </c>
-      <c r="AR80" s="1">
-        <v>0</v>
-      </c>
-      <c r="AS80" s="1">
-        <v>0</v>
-      </c>
-      <c r="AT80" s="1">
-        <v>0</v>
-      </c>
-      <c r="AU80" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV80" s="1">
-        <v>0</v>
-      </c>
-      <c r="AW80" s="1">
-        <v>0</v>
-      </c>
-      <c r="AX80" s="1">
-        <v>0</v>
-      </c>
-      <c r="AY80" s="1">
-        <v>0</v>
-      </c>
-      <c r="AZ80" s="1">
-        <v>0</v>
-      </c>
-      <c r="BA80" s="1">
-        <v>0</v>
-      </c>
-      <c r="BB80" s="1">
-        <v>0</v>
-      </c>
-      <c r="BC80" s="1">
-        <v>0</v>
-      </c>
-      <c r="BD80" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE80" s="1">
-        <v>0</v>
-      </c>
-      <c r="BF80" s="1">
-        <v>0</v>
-      </c>
-      <c r="BG80" s="1">
-        <v>0</v>
-      </c>
-      <c r="BH80" s="1">
-        <v>0</v>
-      </c>
-      <c r="BI80" s="1">
-        <v>0</v>
-      </c>
-      <c r="BJ80" s="1">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="AQ80" s="14">
+        <v>1.5898932920730401E-7</v>
+      </c>
+      <c r="AR80" s="14">
+        <v>7.9494664603652095E-8</v>
+      </c>
+      <c r="AS80" s="14">
+        <v>7.9494664603652095E-8</v>
+      </c>
+      <c r="AT80" s="14">
+        <v>1.5898932920730401E-7</v>
+      </c>
+      <c r="AU80" s="14">
+        <v>1.5898932920730401E-7</v>
+      </c>
+      <c r="AV80" s="14">
+        <v>1.5898932920730401E-7</v>
+      </c>
+      <c r="AW80" s="14">
+        <v>1.5898932920730401E-7</v>
+      </c>
+      <c r="AX80" s="14">
+        <v>3.1797865841460801E-7</v>
+      </c>
+      <c r="AY80" s="14">
+        <v>1.5898932920730401E-7</v>
+      </c>
+      <c r="AZ80" s="14">
+        <v>2.38483993810956E-7</v>
+      </c>
+      <c r="BA80" s="14">
+        <v>2.38483993810956E-7</v>
+      </c>
+      <c r="BB80" s="14">
+        <v>2.38483993810956E-7</v>
+      </c>
+      <c r="BC80" s="14">
+        <v>2.38483993810956E-7</v>
+      </c>
+      <c r="BD80" s="14">
+        <v>2.38483993810956E-7</v>
+      </c>
+      <c r="BE80" s="14">
+        <v>2.38483993810956E-7</v>
+      </c>
+      <c r="BF80" s="14">
+        <v>2.38483993810956E-7</v>
+      </c>
+      <c r="BG80" s="14">
+        <v>2.38483993810956E-7</v>
+      </c>
+      <c r="BH80" s="14">
+        <v>3.1797865841460801E-7</v>
+      </c>
+      <c r="BI80" s="14">
+        <v>2.38483993810956E-7</v>
+      </c>
+      <c r="BJ80" s="14">
+        <v>2.38483993810956E-7</v>
       </c>
     </row>
     <row r="81" spans="1:62" x14ac:dyDescent="0.25">
@@ -20971,14 +20971,14 @@
       <c r="AK81" s="1">
         <v>6.6666666666666671E-3</v>
       </c>
-      <c r="AM81" s="1">
-        <v>8.7385879431639543E-12</v>
-      </c>
-      <c r="AN81" s="1">
-        <v>2.7108299939042762E-5</v>
+      <c r="AM81" s="14">
+        <v>8.7385879431639493E-9</v>
+      </c>
+      <c r="AN81" s="14">
+        <v>6.9999999999999999E-6</v>
       </c>
       <c r="AO81" s="1">
-        <v>8.8918700418838323</v>
+        <v>6</v>
       </c>
       <c r="AQ81" s="1">
         <v>3.1797865841460859E-7</v>
@@ -21138,14 +21138,14 @@
       <c r="AK82" s="1">
         <v>0.31111111111111112</v>
       </c>
-      <c r="AM82" s="1">
-        <v>2.3573518957676141E-8</v>
+      <c r="AM82" s="14">
+        <v>1.3357351895767599E-7</v>
       </c>
       <c r="AN82" s="1">
         <v>3.8555482629656359E-6</v>
       </c>
       <c r="AO82" s="1">
-        <v>0.57824248951054025</v>
+        <v>0.6</v>
       </c>
       <c r="AQ82" s="1">
         <v>2.22585060890226E-6</v>
@@ -21466,14 +21466,14 @@
       <c r="AK84" s="1">
         <v>0.59333333333333338</v>
       </c>
-      <c r="AM84" s="1">
-        <v>7.818683739643212E-9</v>
-      </c>
-      <c r="AN84" s="1">
-        <v>9.5714514558327261E-6</v>
+      <c r="AM84" s="14">
+        <v>8.9999999999999999E-8</v>
+      </c>
+      <c r="AN84" s="14">
+        <v>8.8000000000000004E-6</v>
       </c>
       <c r="AO84" s="1">
-        <v>1.0917157584933179</v>
+        <v>1.2</v>
       </c>
       <c r="AQ84" s="1">
         <v>4.6106905470118257E-6</v>
@@ -21800,14 +21800,14 @@
       <c r="AK86" s="1">
         <v>1.1666666666666671E-2</v>
       </c>
-      <c r="AM86" s="1">
-        <v>5.5624520000987312E-8</v>
+      <c r="AM86" s="14">
+        <v>5.5624520000987299E-8</v>
       </c>
       <c r="AN86" s="1">
-        <v>1.098716933886791E-5</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="AO86" s="1">
-        <v>9.3226192441084752</v>
+        <v>5</v>
       </c>
       <c r="AQ86" s="1">
         <v>1.589893292073043E-7</v>

</xml_diff>